<commit_message>
Matplotlib completed and started seaborn
</commit_message>
<xml_diff>
--- a/Matplotlib/expense3.xlsx
+++ b/Matplotlib/expense3.xlsx
@@ -16,7 +16,7 @@
   <definedNames>
     <definedName name="Slicer_Payment_Mode">#N/A</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
   <pivotCaches>
     <pivotCache cacheId="0" r:id="rId6"/>
   </pivotCaches>
@@ -934,11 +934,11 @@
         <c:dLbls/>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="117894144"/>
-        <c:axId val="117777152"/>
+        <c:axId val="115928064"/>
+        <c:axId val="115811072"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="117894144"/>
+        <c:axId val="115928064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -979,14 +979,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="117777152"/>
+        <c:crossAx val="115811072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="117777152"/>
+        <c:axId val="115811072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1035,7 +1035,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="117894144"/>
+        <c:crossAx val="115928064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2546,14 +2546,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.6">
@@ -2740,7 +2739,7 @@
         <v>50</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -2791,7 +2790,7 @@
         <v>120</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:5">

</xml_diff>